<commit_message>
tests have been ran
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadeg\Documents\EPFL\ma1\ENV-540\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63740A5E-41A1-4F05-8946-31CED7256B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA1F203-E67B-4BA1-9803-7D557D8F9B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
   <si>
     <t>optimizer</t>
   </si>
@@ -90,9 +90,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>same as before but different accuracy ??</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -113,13 +110,59 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>more transf.</t>
+  </si>
+  <si>
+    <t>IoU</t>
+  </si>
+  <si>
+    <t>mIoU</t>
+  </si>
+  <si>
+    <t>Pool</t>
+  </si>
+  <si>
+    <t>Grass</t>
+  </si>
+  <si>
+    <t>Vehicule</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Building 
+flooded</t>
+  </si>
+  <si>
+    <t>Building 
+non-flooded</t>
+  </si>
+  <si>
+    <t>Road 
+flooded</t>
+  </si>
+  <si>
+    <t>Road 
+non-flooded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,8 +191,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -168,8 +231,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -226,11 +295,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -280,9 +387,50 @@
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -560,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M21"/>
+  <dimension ref="B2:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="N2" zoomScale="74" workbookViewId="0">
+      <selection activeCell="AD25" sqref="AD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,10 +719,13 @@
     <col min="1" max="8" width="10.6328125" style="1"/>
     <col min="9" max="9" width="10.6328125" style="12"/>
     <col min="10" max="13" width="10.6328125" style="2"/>
-    <col min="14" max="16384" width="10.6328125" style="1"/>
+    <col min="14" max="15" width="10.6328125" style="1"/>
+    <col min="16" max="25" width="12.6328125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="10.6328125" style="2"/>
+    <col min="27" max="16384" width="10.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:26" s="7" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
@@ -594,7 +745,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>3</v>
@@ -611,8 +762,23 @@
       <c r="M2" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="P2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -632,10 +798,10 @@
         <v>0.01</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2">
         <v>0.72870000000000001</v>
@@ -650,7 +816,7 @@
         <v>0.44450000000000001</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -670,10 +836,10 @@
         <v>1E-3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2">
         <v>0.69130000000000003</v>
@@ -688,7 +854,7 @@
         <v>0.30049999999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
@@ -708,10 +874,10 @@
         <v>0.01</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="2">
         <v>0.50980000000000003</v>
@@ -726,7 +892,7 @@
         <v>0.1774</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
@@ -746,10 +912,10 @@
         <v>1E-3</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2">
         <v>0.59650000000000003</v>
@@ -764,7 +930,7 @@
         <v>0.15770000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -784,10 +950,10 @@
         <v>0.01</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" s="2">
         <v>0.70899999999999996</v>
@@ -802,7 +968,7 @@
         <v>0.52659999999999996</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -822,10 +988,10 @@
         <v>0.01</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="2">
         <v>0.63770000000000004</v>
@@ -839,23 +1005,78 @@
       <c r="M8" s="5">
         <v>0.61129999999999995</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="P8" s="2">
+        <v>0.71974619500000003</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.68471334800000005</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.78729477699999995</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1.5691197199999999E-4</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.83350483900000005</v>
+      </c>
+      <c r="Z8" s="2">
+        <f>AVERAGE(P8:X8)</f>
+        <v>0.50423601182866673</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.75990000000000002</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.57040000000000002</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.78249999999999997</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.53769999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="1">
         <v>30</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="1">
         <v>8</v>
       </c>
       <c r="F10" s="1">
@@ -865,25 +1086,25 @@
         <v>0.01</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="2">
-        <v>0.75990000000000002</v>
+        <v>0.1147</v>
       </c>
       <c r="K10" s="2">
-        <v>0.57040000000000002</v>
+        <v>0.22539999999999999</v>
       </c>
       <c r="L10" s="2">
-        <v>0.78249999999999997</v>
+        <v>0.1447</v>
       </c>
       <c r="M10" s="2">
-        <v>0.53769999999999996</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.23300000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -903,25 +1124,25 @@
         <v>0.01</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="J11" s="2">
-        <v>0.1147</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="K11" s="2">
-        <v>0.22539999999999999</v>
+        <v>0.14610000000000001</v>
       </c>
       <c r="L11" s="2">
-        <v>0.1447</v>
+        <v>0.55420000000000003</v>
       </c>
       <c r="M11" s="2">
-        <v>0.23300000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -937,29 +1158,29 @@
       <c r="F12" s="1">
         <v>20</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="4">
         <v>0.01</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>21</v>
+      <c r="H12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>20</v>
       </c>
       <c r="J12" s="2">
-        <v>0.58330000000000004</v>
+        <v>0.79059999999999997</v>
       </c>
       <c r="K12" s="2">
-        <v>0.14610000000000001</v>
+        <v>0.55100000000000005</v>
       </c>
       <c r="L12" s="2">
-        <v>0.55420000000000003</v>
-      </c>
-      <c r="M12" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.7873</v>
+      </c>
+      <c r="M12" s="16">
+        <v>0.5554</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
@@ -972,32 +1193,33 @@
       <c r="E13" s="1">
         <v>8</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.79059999999999997</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.55100000000000005</v>
+      <c r="J13" s="5">
+        <v>0.84179999999999999</v>
+      </c>
+      <c r="K13" s="16">
+        <v>0.62949999999999995</v>
       </c>
       <c r="L13" s="2">
-        <v>0.7873</v>
-      </c>
-      <c r="M13" s="16">
-        <v>0.5554</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.80959999999999999</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.53159999999999996</v>
+      </c>
+      <c r="P13" s="23"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1010,8 +1232,8 @@
       <c r="E14" s="1">
         <v>8</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>15</v>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="G14" s="4">
         <v>0.01</v>
@@ -1020,22 +1242,22 @@
         <v>13</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0.84179999999999999</v>
+        <v>18</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0.82140000000000002</v>
       </c>
       <c r="K14" s="16">
-        <v>0.62949999999999995</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="L14" s="2">
-        <v>0.80959999999999999</v>
+        <v>0.80310000000000004</v>
       </c>
       <c r="M14" s="2">
-        <v>0.53159999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.52129999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1049,31 +1271,31 @@
         <v>8</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="4">
-        <v>0.01</v>
+        <v>14</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1E-3</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="16">
-        <v>0.82140000000000002</v>
-      </c>
-      <c r="K15" s="16">
-        <v>0.60299999999999998</v>
+        <v>20</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.80059999999999998</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.55459999999999998</v>
       </c>
       <c r="L15" s="2">
-        <v>0.80310000000000004</v>
+        <v>0.8165</v>
       </c>
       <c r="M15" s="2">
-        <v>0.52129999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.54020000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1086,32 +1308,66 @@
       <c r="E16" s="1">
         <v>8</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="4">
         <v>1E-3</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J16" s="2">
-        <v>0.80059999999999998</v>
+        <v>0.80530000000000002</v>
       </c>
       <c r="K16" s="2">
-        <v>0.55459999999999998</v>
+        <v>0.58089999999999997</v>
       </c>
       <c r="L16" s="2">
-        <v>0.8165</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0.54020000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.83120000000000005</v>
+      </c>
+      <c r="M16" s="16">
+        <v>0.59209999999999996</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0.38288823999999999</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0.75064887999999996</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.39212706000000003</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0.65612282</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0.75963497999999996</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0.59874218000000001</v>
+      </c>
+      <c r="W16" s="2">
+        <v>0</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0.8055504</v>
+      </c>
+      <c r="Z16" s="2">
+        <f>AVERAGE(P16:X16)</f>
+        <v>0.39335157333333332</v>
+      </c>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1125,31 +1381,25 @@
         <v>8</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="4">
-        <v>1E-3</v>
+        <v>14</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1E-4</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="16">
-        <v>0.80530000000000002</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0.58089999999999997</v>
-      </c>
-      <c r="L17" s="16">
-        <v>0.83120000000000005</v>
-      </c>
-      <c r="M17" s="16">
-        <v>0.59209999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.78669999999999995</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.39710000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:26" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1163,7 +1413,7 @@
         <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="4">
         <v>1E-4</v>
@@ -1172,16 +1422,55 @@
         <v>13</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.74860000000000004</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.49330000000000002</v>
       </c>
       <c r="L18" s="2">
-        <v>0.78669999999999995</v>
+        <v>0.78159999999999996</v>
       </c>
       <c r="M18" s="2">
-        <v>0.39710000000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.35">
+        <v>0.45169999999999999</v>
+      </c>
+      <c r="P18" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="R18" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="T18" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="U18" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="V18" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="W18" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="X18" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y18" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z18" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1191,52 +1480,136 @@
       <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="1">
-        <v>8</v>
+      <c r="E19" s="3">
+        <v>12</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="3">
-        <v>1E-4</v>
+        <v>14</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1E-3</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.74860000000000004</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.49330000000000002</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0.78159999999999996</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0.45169999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="I21" s="15" t="s">
+      <c r="I19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="6">
-        <f>MAX(J3:J18)</f>
+      <c r="J19" s="18">
+        <v>0.81469999999999998</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0.59470000000000001</v>
+      </c>
+      <c r="L19" s="20">
+        <v>0.83189999999999997</v>
+      </c>
+      <c r="M19" s="21">
+        <v>0.5554</v>
+      </c>
+      <c r="N19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="24">
+        <v>0.28053826999999998</v>
+      </c>
+      <c r="R19" s="24">
+        <v>0.60653701999999998</v>
+      </c>
+      <c r="S19" s="24">
+        <v>0.29389916999999999</v>
+      </c>
+      <c r="T19" s="24">
+        <v>0.66857491000000002</v>
+      </c>
+      <c r="U19" s="24">
+        <v>0.78571497999999995</v>
+      </c>
+      <c r="V19" s="24">
+        <v>0.64723949000000003</v>
+      </c>
+      <c r="W19" s="24">
+        <v>0</v>
+      </c>
+      <c r="X19" s="24">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="28">
+        <v>0.82250186000000003</v>
+      </c>
+      <c r="Z19" s="2">
+        <f t="shared" ref="Z19" si="0">AVERAGE(P19:X19)</f>
+        <v>0.36472264888888889</v>
+      </c>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="4">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.81359999999999999</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0.58579999999999999</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0.8105</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0.56830000000000003</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y20" s="29"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="E21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="I22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="6">
+        <f>MAX(J3:J17)</f>
         <v>0.84179999999999999</v>
       </c>
-      <c r="K21" s="6">
-        <f>MAX(K3:K18)</f>
+      <c r="K22" s="6">
+        <f>MAX(K3:K17)</f>
         <v>0.67169999999999996</v>
       </c>
-      <c r="L21" s="6">
-        <f>MAX(L3:L18)</f>
+      <c r="L22" s="6">
+        <f>MAX(L3:L17)</f>
         <v>0.86250000000000004</v>
       </c>
-      <c r="M21" s="6">
-        <f>MAX(M3:M18)</f>
+      <c r="M22" s="6">
+        <f>MAX(M3:M17)</f>
         <v>0.61129999999999995</v>
       </c>
     </row>

</xml_diff>